<commit_message>
updated code with corrected interactions, model selection
</commit_message>
<xml_diff>
--- a/InteractionTracker_EDL.xlsx
+++ b/InteractionTracker_EDL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F004SPC\Documents\GitHub\FracFarmVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B77E9E-D28B-4403-B9CC-C37BFCD1A1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF0263A-378A-4934-876A-C53F5A821CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CC463D56-13DA-BD4B-A589-490BED5699D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
   <si>
     <t>propM (logit)</t>
   </si>
@@ -98,13 +98,58 @@
     <t>yes/no</t>
   </si>
   <si>
-    <t xml:space="preserve">yes </t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>maybe/yes</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>popM(logit): Caitlin</t>
+  </si>
+  <si>
+    <t>POM Caitlin</t>
+  </si>
+  <si>
+    <t>mgMAOM:Caitlin</t>
+  </si>
+  <si>
+    <t>MAOM only</t>
+  </si>
+  <si>
+    <t>yes to all</t>
+  </si>
+  <si>
+    <t>mang</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>7 terms</t>
+  </si>
+  <si>
+    <t>texture*ppt*tmeanC</t>
+  </si>
+  <si>
+    <t>10 x 20 terms</t>
+  </si>
+  <si>
+    <t>number of samples</t>
+  </si>
+  <si>
+    <t>graphic exploration</t>
+  </si>
+  <si>
+    <t>biologically meaningful</t>
+  </si>
+  <si>
+    <t>interesting from a management  perspective</t>
   </si>
 </sst>
 </file>
@@ -128,12 +173,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,11 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,30 +539,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200B55A7-A47B-4A48-81FD-109B3445001F}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -523,37 +587,76 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
@@ -565,22 +668,40 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -593,50 +714,101 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -649,36 +821,75 @@
       <c r="D11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="H13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -691,8 +902,17 @@
       <c r="D14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -705,8 +925,17 @@
       <c r="D15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -718,6 +947,69 @@
       </c>
       <c r="D16" t="s">
         <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>